<commit_message>
1.qr code 圖片補齊(80) 2.scrollbar:true
</commit_message>
<xml_diff>
--- a/store.xlsx
+++ b/store.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-12" yWindow="-12" windowWidth="10956" windowHeight="10128"/>
+    <workbookView xWindow="-12" yWindow="-12" windowWidth="10956" windowHeight="10128" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="3" r:id="rId1"/>
@@ -1371,7 +1371,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
@@ -3907,7 +3907,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A80"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>